<commit_message>
Added LCD but not working
</commit_message>
<xml_diff>
--- a/STM32F103C8T6_Pinout_Wiring.xlsx
+++ b/STM32F103C8T6_Pinout_Wiring.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="90">
   <si>
     <t>Pin_Name</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>LCD_E</t>
+  </si>
+  <si>
+    <t>LED #2</t>
   </si>
 </sst>
 </file>
@@ -413,14 +416,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -431,18 +443,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -452,13 +452,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1079,784 +1082,854 @@
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="19" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="19" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="20"/>
-      <c r="K4" s="21"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="8"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="9" t="s">
+      <c r="C5" s="15"/>
+      <c r="D5" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="14"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="11"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="11"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="14"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="11"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>4</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="11"/>
     </row>
     <row r="9" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>5</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="6" t="s">
+      <c r="C9" s="15"/>
+      <c r="D9" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="14"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="11"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>6</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="6" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="14"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="11"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>7</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="6" t="s">
+      <c r="C11" s="15"/>
+      <c r="D11" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="14"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="11"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>8</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="6" t="s">
+      <c r="C12" s="15"/>
+      <c r="D12" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="14"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="11"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>9</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="6" t="s">
+      <c r="C13" s="15"/>
+      <c r="D13" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="14"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="11"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>10</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="6" t="s">
+      <c r="C14" s="15"/>
+      <c r="D14" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="14"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="11"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>11</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="6" t="s">
+      <c r="C15" s="15"/>
+      <c r="D15" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="14"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="11"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>12</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="6" t="s">
+      <c r="C16" s="15"/>
+      <c r="D16" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="14"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="11"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>13</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="6" t="s">
+      <c r="C17" s="15"/>
+      <c r="D17" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="14"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="11"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>14</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="6" t="s">
+      <c r="C18" s="15"/>
+      <c r="D18" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="14"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="11"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>15</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="6" t="s">
+      <c r="C19" s="15"/>
+      <c r="D19" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="14"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="11"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>16</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="6" t="s">
+      <c r="C20" s="15"/>
+      <c r="D20" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="14"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="11"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>17</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="11"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>18</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="14"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="11"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>19</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="14"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="11"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>20</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="11"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>21</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="11"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>22</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="14"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="11"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>23</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="14"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="11"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>24</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="6" t="s">
+      <c r="C28" s="15"/>
+      <c r="D28" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="14"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="11"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>25</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="6" t="s">
+      <c r="C29" s="15"/>
+      <c r="D29" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="14"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="11"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>26</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="6" t="s">
+      <c r="C30" s="15"/>
+      <c r="D30" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="14"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="11"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>27</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="6" t="s">
+      <c r="C31" s="15"/>
+      <c r="D31" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="14"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="11"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>28</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="6" t="s">
+      <c r="C32" s="15"/>
+      <c r="D32" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="14"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="11"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>29</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="14"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="11"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>30</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="6" t="s">
+      <c r="C34" s="15"/>
+      <c r="D34" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="14"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="11"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>31</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="14"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="11"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>32</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="6" t="s">
+      <c r="C36" s="15"/>
+      <c r="D36" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="14"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="11"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>33</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="6" t="s">
+      <c r="C37" s="15"/>
+      <c r="D37" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="14"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="11"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>34</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="16"/>
-      <c r="D38" s="6" t="s">
+      <c r="C38" s="15"/>
+      <c r="D38" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="14"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="11"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>35</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="16"/>
-      <c r="D39" s="6" t="s">
+      <c r="C39" s="15"/>
+      <c r="D39" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="13"/>
-      <c r="K39" s="14"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="11"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>36</v>
       </c>
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="16"/>
-      <c r="D40" s="6" t="s">
+      <c r="C40" s="15"/>
+      <c r="D40" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="12"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="14"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="11"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>37</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="6" t="s">
+      <c r="C41" s="15"/>
+      <c r="D41" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="13"/>
-      <c r="K41" s="14"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="11"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>38</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="16"/>
-      <c r="D42" s="6" t="s">
+      <c r="C42" s="15"/>
+      <c r="D42" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="13"/>
-      <c r="K42" s="14"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="11"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>39</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="6" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="12"/>
-      <c r="J43" s="13"/>
-      <c r="K43" s="14"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="11"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>40</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="16"/>
-      <c r="D44" s="6" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="13"/>
-      <c r="K44" s="14"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="11"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="126">
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="D33:H33"/>
+    <mergeCell ref="D34:H34"/>
+    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="D25:H25"/>
+    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="D16:H16"/>
+    <mergeCell ref="D17:H17"/>
+    <mergeCell ref="D18:H18"/>
+    <mergeCell ref="D19:H19"/>
+    <mergeCell ref="D20:H20"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="D15:H15"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="D44:H44"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="D12:H12"/>
+    <mergeCell ref="D13:H13"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="I39:K39"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="I42:K42"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="I38:K38"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="D30:H30"/>
+    <mergeCell ref="D31:H31"/>
+    <mergeCell ref="D32:H32"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D43:H43"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D41:H41"/>
+    <mergeCell ref="D42:H42"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D39:H39"/>
+    <mergeCell ref="D40:H40"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D37:H37"/>
+    <mergeCell ref="D38:H38"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D35:H35"/>
+    <mergeCell ref="D36:H36"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="B30:C30"/>
@@ -1881,95 +1954,25 @@
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D39:H39"/>
-    <mergeCell ref="D40:H40"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D37:H37"/>
-    <mergeCell ref="D38:H38"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D35:H35"/>
-    <mergeCell ref="D36:H36"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:G45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D43:H43"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D41:H41"/>
-    <mergeCell ref="D42:H42"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I7:K7"/>
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="I11:K11"/>
     <mergeCell ref="I12:K12"/>
     <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="D44:H44"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="D12:H12"/>
-    <mergeCell ref="D13:H13"/>
-    <mergeCell ref="D14:H14"/>
-    <mergeCell ref="I39:K39"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="I36:K36"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="I38:K38"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="D16:H16"/>
-    <mergeCell ref="D17:H17"/>
-    <mergeCell ref="D18:H18"/>
-    <mergeCell ref="D19:H19"/>
-    <mergeCell ref="D20:H20"/>
-    <mergeCell ref="D21:H21"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="D15:H15"/>
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="D30:H30"/>
-    <mergeCell ref="D31:H31"/>
-    <mergeCell ref="D32:H32"/>
-    <mergeCell ref="D33:H33"/>
-    <mergeCell ref="D34:H34"/>
-    <mergeCell ref="D22:H22"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="D26:H26"/>
-    <mergeCell ref="D27:H27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1981,8 +1984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41:K41"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2003,108 +2006,110 @@
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="19" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="19" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="20"/>
-      <c r="K4" s="21"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="8"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="9" t="s">
+      <c r="C5" s="15"/>
+      <c r="D5" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="14"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="11"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="11"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="14"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="11"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>4</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="J8" s="23"/>
+      <c r="K8" s="24"/>
     </row>
     <row r="9" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>5</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="6" t="s">
+      <c r="C9" s="15"/>
+      <c r="D9" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="20"/>
       <c r="I9" s="22" t="s">
         <v>72</v>
       </c>
@@ -2115,17 +2120,17 @@
       <c r="A10" s="2">
         <v>6</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="6" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="8"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="20"/>
       <c r="I10" s="22" t="s">
         <v>73</v>
       </c>
@@ -2136,17 +2141,17 @@
       <c r="A11" s="2">
         <v>7</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="6" t="s">
+      <c r="C11" s="15"/>
+      <c r="D11" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="8"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20"/>
       <c r="I11" s="22" t="s">
         <v>74</v>
       </c>
@@ -2157,17 +2162,17 @@
       <c r="A12" s="2">
         <v>8</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="6" t="s">
+      <c r="C12" s="15"/>
+      <c r="D12" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="8"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="20"/>
       <c r="I12" s="22" t="s">
         <v>75</v>
       </c>
@@ -2178,17 +2183,17 @@
       <c r="A13" s="2">
         <v>9</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="6" t="s">
+      <c r="C13" s="15"/>
+      <c r="D13" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="8"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="20"/>
       <c r="I13" s="22" t="s">
         <v>76</v>
       </c>
@@ -2199,17 +2204,17 @@
       <c r="A14" s="2">
         <v>10</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="6" t="s">
+      <c r="C14" s="15"/>
+      <c r="D14" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="8"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="20"/>
       <c r="I14" s="22" t="s">
         <v>77</v>
       </c>
@@ -2220,17 +2225,17 @@
       <c r="A15" s="2">
         <v>11</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="6" t="s">
+      <c r="C15" s="15"/>
+      <c r="D15" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="8"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="20"/>
       <c r="I15" s="22" t="s">
         <v>78</v>
       </c>
@@ -2244,17 +2249,17 @@
       <c r="A16" s="2">
         <v>12</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="6" t="s">
+      <c r="C16" s="15"/>
+      <c r="D16" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="8"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="20"/>
       <c r="I16" s="22" t="s">
         <v>79</v>
       </c>
@@ -2265,17 +2270,17 @@
       <c r="A17" s="2">
         <v>13</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="6" t="s">
+      <c r="C17" s="15"/>
+      <c r="D17" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="8"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="20"/>
       <c r="I17" s="22" t="s">
         <v>80</v>
       </c>
@@ -2286,36 +2291,36 @@
       <c r="A18" s="2">
         <v>14</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="6" t="s">
+      <c r="C18" s="15"/>
+      <c r="D18" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="14"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="11"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>15</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="6" t="s">
+      <c r="C19" s="15"/>
+      <c r="D19" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="8"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="20"/>
       <c r="I19" s="22" t="s">
         <v>87</v>
       </c>
@@ -2326,17 +2331,17 @@
       <c r="A20" s="2">
         <v>16</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="6" t="s">
+      <c r="C20" s="15"/>
+      <c r="D20" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="8"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="20"/>
       <c r="I20" s="22" t="s">
         <v>88</v>
       </c>
@@ -2347,18 +2352,18 @@
       <c r="A21" s="2">
         <v>17</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="11"/>
       <c r="M21"/>
       <c r="U21" s="1" t="s">
         <v>70</v>
@@ -2369,157 +2374,157 @@
       <c r="A22" s="3">
         <v>18</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="14"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="11"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>19</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="14"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="11"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>20</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="11"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>21</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="11"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>22</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="14"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="11"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>23</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="14"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="11"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>24</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="6" t="s">
+      <c r="C28" s="15"/>
+      <c r="D28" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="14"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="11"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>25</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="6" t="s">
+      <c r="C29" s="15"/>
+      <c r="D29" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="14"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="11"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>26</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="6" t="s">
+      <c r="C30" s="15"/>
+      <c r="D30" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="8"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="20"/>
       <c r="I30" s="22" t="s">
         <v>81</v>
       </c>
@@ -2530,17 +2535,17 @@
       <c r="A31" s="3">
         <v>27</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="6" t="s">
+      <c r="C31" s="15"/>
+      <c r="D31" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="8"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="20"/>
       <c r="I31" s="22" t="s">
         <v>82</v>
       </c>
@@ -2551,184 +2556,184 @@
       <c r="A32" s="2">
         <v>28</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="6" t="s">
+      <c r="C32" s="15"/>
+      <c r="D32" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="14"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="11"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>29</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="14"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="11"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>30</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="6" t="s">
+      <c r="C34" s="15"/>
+      <c r="D34" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="14"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="11"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>31</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="14"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="11"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>32</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="6" t="s">
+      <c r="C36" s="15"/>
+      <c r="D36" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="14"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="11"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>33</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="6" t="s">
+      <c r="C37" s="15"/>
+      <c r="D37" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="14"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="11"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>34</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="16"/>
-      <c r="D38" s="6" t="s">
+      <c r="C38" s="15"/>
+      <c r="D38" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="14"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="11"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>35</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="16"/>
-      <c r="D39" s="6" t="s">
+      <c r="C39" s="15"/>
+      <c r="D39" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="13"/>
-      <c r="K39" s="14"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="11"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>36</v>
       </c>
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="16"/>
-      <c r="D40" s="6" t="s">
+      <c r="C40" s="15"/>
+      <c r="D40" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="12"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="14"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="11"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>37</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="6" t="s">
+      <c r="C41" s="15"/>
+      <c r="D41" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="8"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="20"/>
       <c r="I41" s="22" t="s">
         <v>85</v>
       </c>
@@ -2739,17 +2744,17 @@
       <c r="A42" s="3">
         <v>38</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="16"/>
-      <c r="D42" s="6" t="s">
+      <c r="C42" s="15"/>
+      <c r="D42" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="8"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="20"/>
       <c r="I42" s="22" t="s">
         <v>86</v>
       </c>
@@ -2760,17 +2765,17 @@
       <c r="A43" s="3">
         <v>39</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="6" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="8"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="20"/>
       <c r="I43" s="22" t="s">
         <v>84</v>
       </c>
@@ -2784,17 +2789,17 @@
       <c r="A44" s="3">
         <v>40</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="16"/>
-      <c r="D44" s="6" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="8"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="20"/>
       <c r="I44" s="22" t="s">
         <v>83</v>
       </c>
@@ -2802,38 +2807,116 @@
       <c r="K44" s="24"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79"/>
     </row>
   </sheetData>
   <mergeCells count="126">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:H44"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:H42"/>
+    <mergeCell ref="I42:K42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:H43"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:H40"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:H41"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:H38"/>
+    <mergeCell ref="I38:K38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:H39"/>
+    <mergeCell ref="I39:K39"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:H36"/>
+    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:H37"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:H34"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:H35"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:H32"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:H33"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:H30"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:H31"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:H25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:H16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:H17"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:H15"/>
+    <mergeCell ref="I15:K15"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:H12"/>
     <mergeCell ref="I12:K12"/>
@@ -2846,102 +2929,24 @@
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:H11"/>
     <mergeCell ref="I11:K11"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:H16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:H17"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:H14"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:H15"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:H21"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:H19"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:H22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:H26"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:H32"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:H33"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:H30"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:H31"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:H36"/>
-    <mergeCell ref="I36:K36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:H37"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:H34"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:H35"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:H40"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:H41"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:H38"/>
-    <mergeCell ref="I38:K38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:H39"/>
-    <mergeCell ref="I39:K39"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:H44"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:G45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:H42"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:H43"/>
-    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="I8:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>